<commit_message>
exercícios da lista N1 e material dos proximos exercicios
</commit_message>
<xml_diff>
--- a/IES300-Engenharia de Software III/Lista de Exercícios/ListaN1_CasoDeUsoTextual.xlsx
+++ b/IES300-Engenharia de Software III/Lista de Exercícios/ListaN1_CasoDeUsoTextual.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nome do caso de uso" sheetId="1" state="visible" r:id="rId2"/>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Cliente informa dados para secretário.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cliente informacpf e data de nascimento para secretário.</t>
+    <t xml:space="preserve">Cliente informa cpf e data de nascimento para secretário.</t>
   </si>
   <si>
     <t xml:space="preserve">Secretário verifica se cliente já está cadastrado no sistema. Se não, segue o fluxo principal. Se sim, vai para o alternativo.</t>
@@ -2976,8 +2976,8 @@
   </sheetPr>
   <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M35" activeCellId="0" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10458,7 +10458,7 @@
   </sheetPr>
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>